<commit_message>
fix: update data validation
</commit_message>
<xml_diff>
--- a/gestor/mackensina_importacao_alunos.xlsx
+++ b/gestor/mackensina_importacao_alunos.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Downloads/mackensina_importacao_aluno_equipe_escolar_2024 (5)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cunha\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1E2071-2899-4F45-8D48-FE1DFBE49BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="ofLcP58swWGevM6JFy2rGpVDLJ+X0P5nEKOwA7Mvzjy05pk2ZknIgvbUdZ8I+6/v0vhzfGDT0AbWody0dnccbA==" workbookSaltValue="Ik7d3C2vQGoyNeP8x8xIDw==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33955E93-3210-4F41-BC9F-E8C3BE80504A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="iGSTzoRHm8eRIRTneR3I9/s01HKAol/22TpvHfNyEqR/YxUF7fxTgWRqDngWJaRbNAz3v/Eq/oE+bDAkJ+25FQ==" workbookSaltValue="woUCbr302hXPhtsBGimIzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="740" windowWidth="38960" windowHeight="22600" xr2:uid="{83A79F5F-691D-4D34-B56F-DF3F271EF920}"/>
+    <workbookView xWindow="2190" yWindow="1050" windowWidth="25425" windowHeight="14430" xr2:uid="{83A79F5F-691D-4D34-B56F-DF3F271EF920}"/>
   </bookViews>
   <sheets>
     <sheet name="Alunos" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Alunos!$A$6:$I$6</definedName>
-    <definedName name="EducacaoInfantil">Ajuda!$B$3:$B$6</definedName>
-    <definedName name="EnsinoMedio">Ajuda!$B$16:$B$18</definedName>
-    <definedName name="EtapasEnsino">Ajuda!$A$3:$A$18</definedName>
-    <definedName name="FundamentalFinais">Ajuda!$B$12:$B$15</definedName>
-    <definedName name="FundamentalIniciais">Ajuda!$B$7:$B$11</definedName>
+    <definedName name="Etapa">Ajuda!$A$3:$A$19</definedName>
+    <definedName name="Serie">Ajuda!$B$3:$B$19</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -46,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Alunos</t>
   </si>
@@ -328,6 +325,12 @@
   </si>
   <si>
     <t>Ensino Fundamental - Anos Finais</t>
+  </si>
+  <si>
+    <t>Extracurricular</t>
+  </si>
+  <si>
+    <t>Selecione na coluna "Série" um dos itens abaixo.</t>
   </si>
 </sst>
 </file>
@@ -690,7 +693,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -717,7 +720,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -1016,25 +1019,25 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="158" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="158" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="40" style="6" customWidth="1"/>
-    <col min="3" max="4" width="35.5" style="6" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="35.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="6" customWidth="1"/>
     <col min="6" max="6" width="35" style="6" customWidth="1"/>
-    <col min="7" max="7" width="35.1640625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="32.5" style="6" customWidth="1"/>
-    <col min="9" max="9" width="32.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="32.42578125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="32.7109375" style="6" customWidth="1"/>
     <col min="10" max="10" width="0" style="5" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1640625" style="5" hidden="1"/>
+    <col min="11" max="16384" width="9.140625" style="5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -1047,7 +1050,7 @@
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>11</v>
       </c>
@@ -1060,7 +1063,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
@@ -1073,7 +1076,7 @@
       <c r="H3" s="21"/>
       <c r="I3" s="22"/>
     </row>
-    <row r="4" spans="1:9" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>13</v>
       </c>
@@ -1086,7 +1089,7 @@
       <c r="H4" s="23"/>
       <c r="I4" s="23"/>
     </row>
-    <row r="5" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>0</v>
       </c>
@@ -1101,7 +1104,7 @@
       <c r="H5" s="15"/>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
@@ -1130,7 +1133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1140,19 +1143,19 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E9" s="9"/>
       <c r="G9" s="9"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="1LZSVLBVaVePSLF1/HBFbXVpRTIVLdm1xLFDTn1VXuy4raTcDrc1AK4pLCq7IN4/jrLxhpiEX+EHCZoKsJM+ew==" saltValue="+o83TwUhtPN4tC83SvRN6A==" spinCount="100000" sheet="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="tI18JcKj1syNiaRiSZgTuvlK82WRcTM6BXeYo+5hgTY4jJWN7qOCVWThR1LJ4jC1pjQwJPIV57gW7WgRHW9WfA==" saltValue="wXeCoU2K/wDUlvvOZN0qvA==" spinCount="100000" sheet="1" selectLockedCells="1" autoFilter="0"/>
   <dataConsolidate/>
   <mergeCells count="5">
     <mergeCell ref="A2:I2"/>
@@ -1177,29 +1180,23 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Matrícula Inválida" error="Não colocar caracteres especiais no campo Matrcula, somente letras e números." sqref="A7:A1048576" xr:uid="{26122C4D-FBBC-48A7-8521-C98AC7DECC9E}">
       <formula1>AND( ISERR(FIND("!",A7)), ISERR(FIND("@",A7)), ISERR(FIND("#",A7)), ISERR(FIND("$",A7)), ISERR(FIND("%",A7)), ISERR(FIND("&amp;",A7)), ISERR(FIND("*",A7)),ISERR(FIND(",",A7)),ISERR(FIND(".",A7)))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{41DA1254-1799-0748-B786-6D4466F55DD0}">
-      <formula1>EtapasEnsino</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D1048576" xr:uid="{9CC907AB-E461-4241-9781-C3E4E53DC6F4}">
+      <formula1>Serie</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D1048576" xr:uid="{9CC907AB-E461-4241-9781-C3E4E53DC6F4}">
-      <formula1>IF(C7="Educação Infantil", EducacaoInfantil, IF(C7="Ensino Fundamental Anos Iniciais", FundamentalIniciais, IF(C7="Ensino Fundamental Anos Finais", FundamentalFinais, IF(C7="Ensino Médio", EnsinoMedio, ""))))</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C1048576" xr:uid="{9B3E84FF-8886-4C82-B67B-D3FA4A20783E}">
+      <formula1>Etapa</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EBCFB93B-C9EB-4879-963E-A7EBA7488AC2}">
           <x14:formula1>
             <xm:f>Ajuda!$A$3:$A$9</xm:f>
           </x14:formula1>
           <xm:sqref>C5:D5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FF46153A-5DE8-4D51-9985-F1B51416181F}">
-          <x14:formula1>
-            <xm:f>Ajuda!$A$3:$A$18</xm:f>
-          </x14:formula1>
-          <xm:sqref>C8:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1212,28 +1209,28 @@
   <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="172" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="172" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.6640625" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" customWidth="1"/>
+    <col min="1" max="1" width="59.7109375" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -1241,7 +1238,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1249,7 +1246,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1257,7 +1254,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -1265,7 +1262,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>34</v>
       </c>
@@ -1273,7 +1270,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
@@ -1281,7 +1278,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
@@ -1289,7 +1286,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -1297,7 +1294,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
@@ -1305,7 +1302,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
@@ -1313,7 +1310,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>35</v>
       </c>
@@ -1321,7 +1318,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
@@ -1329,7 +1326,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>35</v>
       </c>
@@ -1337,7 +1334,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
@@ -1345,7 +1342,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1353,7 +1350,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -1361,11 +1358,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix/ajustes na planilha aluno 1.0.2 | professor 1.0.4
</commit_message>
<xml_diff>
--- a/gestor/mackensina_importacao_alunos.xlsx
+++ b/gestor/mackensina_importacao_alunos.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cunha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\github\sme_images\gestor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33955E93-3210-4F41-BC9F-E8C3BE80504A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="iGSTzoRHm8eRIRTneR3I9/s01HKAol/22TpvHfNyEqR/YxUF7fxTgWRqDngWJaRbNAz3v/Eq/oE+bDAkJ+25FQ==" workbookSaltValue="woUCbr302hXPhtsBGimIzw==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458BE4A8-B083-4A32-BE36-B8BA56CFA338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="l592/576FsPboWtHn0oYFpaUC+4jX3h7FPjILJlPxppX/XchOevZEqELb3hax2/853eQf+CVUC0tKYvrt7b1GQ==" workbookSaltValue="VhcpQDMQ1SdSBB6XmUpiuQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="2190" yWindow="1050" windowWidth="25425" windowHeight="14430" xr2:uid="{83A79F5F-691D-4D34-B56F-DF3F271EF920}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{83A79F5F-691D-4D34-B56F-DF3F271EF920}"/>
   </bookViews>
   <sheets>
     <sheet name="Alunos" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Alunos!$A$6:$I$6</definedName>
-    <definedName name="Etapa">Ajuda!$A$3:$A$19</definedName>
+    <definedName name="Etapa">Ajuda!$A$3:$A$18</definedName>
     <definedName name="Serie">Ajuda!$B$3:$B$19</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>Alunos</t>
   </si>
@@ -180,50 +180,6 @@
   </si>
   <si>
     <t>LEIA COM ATENÇÃO</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>número de Matrícula</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ou </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Registro Acadêmico</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> corresponde ao código exclusivo atribuído a cada aluno. Caso sua escola não disponha dessas informações, favor gerar um código único para cada aluno. 
-Evite retrabalho, não altere a ordenação das colunas. Caso contrário, o sistema não reconhecerá as informações. Preste atenção aos campos obrigatórios para garantir uma importação bem-sucedida.  </t>
-    </r>
   </si>
   <si>
     <r>
@@ -318,9 +274,6 @@
     </r>
   </si>
   <si>
-    <t>(v 1.0.1)</t>
-  </si>
-  <si>
     <t>Ensino Fundamental - Anos Iniciais</t>
   </si>
   <si>
@@ -331,13 +284,69 @@
   </si>
   <si>
     <t>Selecione na coluna "Série" um dos itens abaixo.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>número de Matrícula</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ou </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Registro Acadêmico</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> corresponde ao código exclusivo atribuído a cada aluno. Caso sua escola não disponha dessas informações, favor gerar um código único para cada aluno. 
+Evite retrabalho, não altere a ordenação das colunas, não deixar linhas em branco. Caso contrário, o sistema não reconhecerá as informações. Preste atenção aos campos obrigatórios para garantir uma importação bem-sucedida.  </t>
+    </r>
+  </si>
+  <si>
+    <t>Aluno Exemplo</t>
+  </si>
+  <si>
+    <t>responsavel.exemplo@mackensina.br</t>
+  </si>
+  <si>
+    <t>Responsável Exemplo</t>
+  </si>
+  <si>
+    <t>(v 1.0.2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,14 +376,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFE1001E"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -383,14 +384,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -426,6 +419,29 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFE1001E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -476,7 +492,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -555,19 +571,6 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="0" tint="-4.9989318521683403E-2"/>
       </left>
       <right/>
@@ -624,32 +627,19 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -658,8 +648,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -667,33 +675,30 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -720,9 +725,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -760,7 +765,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -866,7 +871,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1008,7 +1013,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1017,145 +1022,145 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B0709D5-2C07-4FAE-815D-B92E40AA1F2F}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="158" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="40" style="6" customWidth="1"/>
-    <col min="3" max="4" width="35.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="35" style="6" customWidth="1"/>
-    <col min="7" max="7" width="35.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="32.42578125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="32.7109375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="0" style="5" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5" hidden="1"/>
+    <col min="1" max="1" width="19.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="40" style="4" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18" style="4" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="35" style="4" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="32.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="32.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="0" style="3" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="3" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+        <v>40</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="23"/>
+    </row>
+    <row r="4" spans="1:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22"/>
-    </row>
-    <row r="4" spans="1:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+    </row>
+    <row r="5" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-    </row>
-    <row r="5" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="9"/>
+      <c r="D7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="tI18JcKj1syNiaRiSZgTuvlK82WRcTM6BXeYo+5hgTY4jJWN7qOCVWThR1LJ4jC1pjQwJPIV57gW7WgRHW9WfA==" saltValue="wXeCoU2K/wDUlvvOZN0qvA==" spinCount="100000" sheet="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="8XLHYbvKC1hqKApTJQY8cJyAPHV6UnD2gvrcxkRWMS1s2gJJePLTR/uFOzRezM1B4jMgx028Uuq98GR7dhWwag==" saltValue="yJt9uxLI61g9skgK6PD9NA==" spinCount="100000" sheet="1" insertRows="0" deleteRows="0" selectLockedCells="1" autoFilter="0"/>
   <dataConsolidate/>
   <mergeCells count="5">
     <mergeCell ref="A2:I2"/>
@@ -1164,18 +1169,12 @@
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:I4"/>
   </mergeCells>
-  <dataValidations count="7">
+  <dataValidations count="4">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1" xr:uid="{A76CCFB0-948C-4094-9E45-15F0E648A369}">
-      <formula1>ISNUMBER(MATCH("*@*.???*",I7,0))</formula1>
+      <formula1>ISNUMBER(MATCH("*@*.???*",#REF!,0))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Inválido o e-mail" error="Verificar o formato do campo e-mail." sqref="G8:G1048576 I7:I1048576 E7:E12 E14:E1048576" xr:uid="{9243C4DB-B85E-483F-B6DF-3B61EC60DE85}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Inválido o e-mail" error="Verificar o formato do campo e-mail." sqref="G7:G1048576 I7:I1048576 E7:E1048576" xr:uid="{9243C4DB-B85E-483F-B6DF-3B61EC60DE85}">
       <formula1>ISNUMBER(MATCH("*@*.??*",E7,0))</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Inválido o e-mail" error="Verificar o formato do e-mail" sqref="G7" xr:uid="{CA0E596F-1EB3-45F5-AF1C-7889B43195C1}">
-      <formula1>ISNUMBER(MATCH("*@*.???*",B7,0))</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13" xr:uid="{C12B2C4B-079A-449E-BD55-924E53C256CC}">
-      <formula1>"NÃO(ÉERRO(PROCURAR(MINÚSCULA(MID(A6; COLUNA(INDIRETO(""1:"" &amp; NÚM.CARACT(A1))); 1)); ""abcdefghijklmnopqrçstuvwxyz0123456789"")))"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Matrícula Inválida" error="Não colocar caracteres especiais no campo Matrcula, somente letras e números." sqref="A7:A1048576" xr:uid="{26122C4D-FBBC-48A7-8521-C98AC7DECC9E}">
       <formula1>AND( ISERR(FIND("!",A7)), ISERR(FIND("@",A7)), ISERR(FIND("#",A7)), ISERR(FIND("$",A7)), ISERR(FIND("%",A7)), ISERR(FIND("&amp;",A7)), ISERR(FIND("*",A7)),ISERR(FIND(",",A7)),ISERR(FIND(".",A7)))</formula1>
@@ -1183,20 +1182,26 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D1048576" xr:uid="{9CC907AB-E461-4241-9781-C3E4E53DC6F4}">
       <formula1>Serie</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C1048576" xr:uid="{9B3E84FF-8886-4C82-B67B-D3FA4A20783E}">
-      <formula1>Etapa</formula1>
-    </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G7" r:id="rId1" xr:uid="{187C41B3-8DC4-4A86-A08A-347BA018C828}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EBCFB93B-C9EB-4879-963E-A7EBA7488AC2}">
           <x14:formula1>
             <xm:f>Ajuda!$A$3:$A$9</xm:f>
           </x14:formula1>
           <xm:sqref>C5:D5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9B3E84FF-8886-4C82-B67B-D3FA4A20783E}">
+          <x14:formula1>
+            <xm:f>Ajuda!$A$3:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>C7:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1209,8 +1214,8 @@
   <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="172" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,154 +1225,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B2" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="4" t="s">
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+      <c r="B9" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+      <c r="B17" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
fix/ajustes de texto nas instruções
</commit_message>
<xml_diff>
--- a/gestor/mackensina_importacao_alunos.xlsx
+++ b/gestor/mackensina_importacao_alunos.xlsx
@@ -8,8 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\github\sme_images\gestor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458BE4A8-B083-4A32-BE36-B8BA56CFA338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="l592/576FsPboWtHn0oYFpaUC+4jX3h7FPjILJlPxppX/XchOevZEqELb3hax2/853eQf+CVUC0tKYvrt7b1GQ==" workbookSaltValue="VhcpQDMQ1SdSBB6XmUpiuQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A55DE22-51E0-4997-A893-B2F44484D81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="SbbH9t/o5HeaVRCp0PFWc+Mi8vx1glt4u01Gb2aeeheUuXZ4u9d9XJkp0Sk+2BkLKAQwf1nWW/I0QD5mY0RHWg==" workbookSaltValue="lYK/x/9PeDwcVuWvwmipLQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{83A79F5F-691D-4D34-B56F-DF3F271EF920}"/>
   </bookViews>
@@ -286,6 +286,18 @@
     <t>Selecione na coluna "Série" um dos itens abaixo.</t>
   </si>
   <si>
+    <t>Aluno Exemplo</t>
+  </si>
+  <si>
+    <t>responsavel.exemplo@mackensina.br</t>
+  </si>
+  <si>
+    <t>Responsável Exemplo</t>
+  </si>
+  <si>
+    <t>(v 1.0.2)</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">O </t>
     </r>
@@ -326,20 +338,8 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> corresponde ao código exclusivo atribuído a cada aluno. Caso sua escola não disponha dessas informações, favor gerar um código único para cada aluno. 
-Evite retrabalho, não altere a ordenação das colunas, não deixar linhas em branco. Caso contrário, o sistema não reconhecerá as informações. Preste atenção aos campos obrigatórios para garantir uma importação bem-sucedida.  </t>
-    </r>
-  </si>
-  <si>
-    <t>Aluno Exemplo</t>
-  </si>
-  <si>
-    <t>responsavel.exemplo@mackensina.br</t>
-  </si>
-  <si>
-    <t>Responsável Exemplo</t>
-  </si>
-  <si>
-    <t>(v 1.0.2)</t>
+Evite retrabalho: não altere a ordenação das colunas e não deixe linhas em branco. Caso contrário, o sistema não reconhecerá as informações. Preste atenção aos campos obrigatórios para garantir uma importação bem-sucedida.  </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1024,7 +1024,7 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1045,7 +1045,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="3" spans="1:9" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
@@ -1144,7 +1144,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>13</v>
@@ -1153,14 +1153,14 @@
         <v>17</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8XLHYbvKC1hqKApTJQY8cJyAPHV6UnD2gvrcxkRWMS1s2gJJePLTR/uFOzRezM1B4jMgx028Uuq98GR7dhWwag==" saltValue="yJt9uxLI61g9skgK6PD9NA==" spinCount="100000" sheet="1" insertRows="0" deleteRows="0" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="NPQYCr2TNUvFzkc/d0SwJlLOA0AcTVGBzIwsxWWbgrt2szxSV6m2L+reNrHycT8CTEMaKWT0x24hN683Ug3qKg==" saltValue="BV/1e1kixq8Fz8WkQOTBFw==" spinCount="100000" sheet="1" insertRows="0" deleteRows="0" selectLockedCells="1" autoFilter="0"/>
   <dataConsolidate/>
   <mergeCells count="5">
     <mergeCell ref="A2:I2"/>

</xml_diff>

<commit_message>
fix/multisseriada adicionado nas lista de series
</commit_message>
<xml_diff>
--- a/gestor/mackensina_importacao_alunos.xlsx
+++ b/gestor/mackensina_importacao_alunos.xlsx
@@ -8,8 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\github\sme_images\gestor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A55DE22-51E0-4997-A893-B2F44484D81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="SbbH9t/o5HeaVRCp0PFWc+Mi8vx1glt4u01Gb2aeeheUuXZ4u9d9XJkp0Sk+2BkLKAQwf1nWW/I0QD5mY0RHWg==" workbookSaltValue="lYK/x/9PeDwcVuWvwmipLQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1B63B2-2528-4FBB-9416-468F4F70EC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="lKHnDmYxGE0yiSCnlmJt55SRFAxOAMRNVpAwJzEqynlD8XKpnDY4xUXtY+yt7CZ7p6BIR+o2EzBgycgkxTkFWg==" workbookSaltValue="V7ta60Kdw4UN1QZoi9AJkA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{83A79F5F-691D-4D34-B56F-DF3F271EF920}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Alunos</t>
   </si>
@@ -340,6 +340,9 @@
       <t xml:space="preserve"> corresponde ao código exclusivo atribuído a cada aluno. Caso sua escola não disponha dessas informações, favor gerar um código único para cada aluno. 
 Evite retrabalho: não altere a ordenação das colunas e não deixe linhas em branco. Caso contrário, o sistema não reconhecerá as informações. Preste atenção aos campos obrigatórios para garantir uma importação bem-sucedida.  </t>
     </r>
+  </si>
+  <si>
+    <t>Multisseriada</t>
   </si>
 </sst>
 </file>
@@ -1024,8 +1027,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,7 +1163,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="NPQYCr2TNUvFzkc/d0SwJlLOA0AcTVGBzIwsxWWbgrt2szxSV6m2L+reNrHycT8CTEMaKWT0x24hN683Ug3qKg==" saltValue="BV/1e1kixq8Fz8WkQOTBFw==" spinCount="100000" sheet="1" insertRows="0" deleteRows="0" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="qtGENAM+Ogz+xhoA10OqZkQcFHrIcG2Jx5v2FNlfiyAMXdoTd5SJljGE13iheFp2Dz5p4oGxm1+IBUH8wVUgzA==" saltValue="a16RHbBi0WeIV8oq6lJP9w==" spinCount="100000" sheet="1" insertRows="0" deleteRows="0" selectLockedCells="1" autoFilter="0"/>
   <dataConsolidate/>
   <mergeCells count="5">
     <mergeCell ref="A2:I2"/>
@@ -1169,7 +1172,7 @@
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:I4"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1" xr:uid="{A76CCFB0-948C-4094-9E45-15F0E648A369}">
       <formula1>ISNUMBER(MATCH("*@*.???*",#REF!,0))</formula1>
     </dataValidation>
@@ -1179,9 +1182,6 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Matrícula Inválida" error="Não colocar caracteres especiais no campo Matrcula, somente letras e números." sqref="A7:A1048576" xr:uid="{26122C4D-FBBC-48A7-8521-C98AC7DECC9E}">
       <formula1>AND( ISERR(FIND("!",A7)), ISERR(FIND("@",A7)), ISERR(FIND("#",A7)), ISERR(FIND("$",A7)), ISERR(FIND("%",A7)), ISERR(FIND("&amp;",A7)), ISERR(FIND("*",A7)),ISERR(FIND(",",A7)),ISERR(FIND(".",A7)))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D1048576" xr:uid="{9CC907AB-E461-4241-9781-C3E4E53DC6F4}">
-      <formula1>Serie</formula1>
-    </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="G7" r:id="rId1" xr:uid="{187C41B3-8DC4-4A86-A08A-347BA018C828}"/>
@@ -1190,7 +1190,13 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9CC907AB-E461-4241-9781-C3E4E53DC6F4}">
+          <x14:formula1>
+            <xm:f>Ajuda!$B$3:$B$21</xm:f>
+          </x14:formula1>
+          <xm:sqref>D7:D1048576</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EBCFB93B-C9EB-4879-963E-A7EBA7488AC2}">
           <x14:formula1>
             <xm:f>Ajuda!$A$3:$A$9</xm:f>
@@ -1215,7 +1221,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,8 +1353,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
+      <c r="B20" s="12" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
removido a validacao do excel
</commit_message>
<xml_diff>
--- a/gestor/mackensina_importacao_alunos.xlsx
+++ b/gestor/mackensina_importacao_alunos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\github\sme_images\gestor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1B63B2-2528-4FBB-9416-468F4F70EC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B19E56-479E-41D4-8A0F-3013BB80EF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="lKHnDmYxGE0yiSCnlmJt55SRFAxOAMRNVpAwJzEqynlD8XKpnDY4xUXtY+yt7CZ7p6BIR+o2EzBgycgkxTkFWg==" workbookSaltValue="V7ta60Kdw4UN1QZoi9AJkA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{83A79F5F-691D-4D34-B56F-DF3F271EF920}"/>
@@ -1027,8 +1027,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" activeCellId="2" sqref="G7:G1048576 I7:I1048576 E7:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,7 +1163,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="qtGENAM+Ogz+xhoA10OqZkQcFHrIcG2Jx5v2FNlfiyAMXdoTd5SJljGE13iheFp2Dz5p4oGxm1+IBUH8wVUgzA==" saltValue="a16RHbBi0WeIV8oq6lJP9w==" spinCount="100000" sheet="1" insertRows="0" deleteRows="0" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="uOpVmOtqZJbGhPcCSFLrat7iE1oyJjjiTtXMf3jQXAPc/eKserCu2np/ckEwrgI7QjM5EGw/9DM/1Ds0JONLBg==" saltValue="eX6iC0ZMVL3bRsEHFvzW6g==" spinCount="100000" sheet="1" insertRows="0" deleteRows="0" selectLockedCells="1" autoFilter="0"/>
   <dataConsolidate/>
   <mergeCells count="5">
     <mergeCell ref="A2:I2"/>
@@ -1176,9 +1176,7 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1" xr:uid="{A76CCFB0-948C-4094-9E45-15F0E648A369}">
       <formula1>ISNUMBER(MATCH("*@*.???*",#REF!,0))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Inválido o e-mail" error="Verificar o formato do campo e-mail." sqref="G7:G1048576 I7:I1048576 E7:E1048576" xr:uid="{9243C4DB-B85E-483F-B6DF-3B61EC60DE85}">
-      <formula1>ISNUMBER(MATCH("*@*.??*",E7,0))</formula1>
-    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Inválido o e-mail" error="Verificar o formato do campo e-mail." sqref="G7:G1048576 I7:I1048576 E7:E1048576" xr:uid="{9243C4DB-B85E-483F-B6DF-3B61EC60DE85}"/>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Matrícula Inválida" error="Não colocar caracteres especiais no campo Matrcula, somente letras e números." sqref="A7:A1048576" xr:uid="{26122C4D-FBBC-48A7-8521-C98AC7DECC9E}">
       <formula1>AND( ISERR(FIND("!",A7)), ISERR(FIND("@",A7)), ISERR(FIND("#",A7)), ISERR(FIND("$",A7)), ISERR(FIND("%",A7)), ISERR(FIND("&amp;",A7)), ISERR(FIND("*",A7)),ISERR(FIND(",",A7)),ISERR(FIND(".",A7)))</formula1>
     </dataValidation>

</xml_diff>